<commit_message>
PROS-7524 SANOFIIN Kpi Update
</commit_message>
<xml_diff>
--- a/Projects/SANOFIIN/Data/Template.xlsx
+++ b/Projects/SANOFIIN/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -442,7 +442,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="41">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -555,51 +555,13 @@
     <t xml:space="preserve">SKUs</t>
   </si>
   <si>
-    <t xml:space="preserve">CHC - Branding (Poster and Glass Door ) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAINCHC18050471
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multibrand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multicategory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Counter Top</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAINCHC17060656
-</t>
+    <t xml:space="preserve">Combiflam ICY HOT 15 gms/30 gms Gel</t>
   </si>
   <si>
     <t xml:space="preserve">Combiflam ICY HOT</t>
   </si>
   <si>
     <t xml:space="preserve">Pain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Window Display</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAINFEX18050480</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allegra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allergy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allegra 120 mg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allegra 180 mg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combiflam ICY HOT 15 gms/30 gms Gel</t>
   </si>
   <si>
     <t xml:space="preserve">Combiflam ICY HOT 35 gms/55 gms Gel</t>
@@ -864,7 +826,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="52">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1019,18 +981,6 @@
     </xf>
     <xf numFmtId="166" fontId="9" fillId="8" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="10" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1065,35 +1015,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
+    <xf numFmtId="164" fontId="16" fillId="10" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="17" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1183,13 +1121,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1453,12 +1391,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="43.8097165991903"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="44.1336032388664"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.2105263157895"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="13" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="21.2105263157895"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="14" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -1545,11 +1483,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="13" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="31.5991902834008"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="13" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="31.8137651821862"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="23.2429149797571"/>
     <col collapsed="false" hidden="false" max="1023" min="7" style="14" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.89068825910931"/>
   </cols>
@@ -1718,16 +1656,16 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="32" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="32" width="37.8137651821862"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="32" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="32" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="32" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="32" width="38.0283400809717"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="32" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="32" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="33" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -1778,20 +1716,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="35" width="32.7773279352227"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="35" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="35" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="35" width="32.9919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="35" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="35" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="14" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -1825,97 +1763,31 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="78.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="29" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="29" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="29" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="42"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="47"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="42"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="47"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="44"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="44"/>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="44"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="39"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="44"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="41"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="41"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A3:A5" type="list">
-      <formula1>"Product Minimum Facings Primary,Product Minimum Facing Secondary "</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1932,20 +1804,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="31.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="34.919028340081"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="35.1336032388664"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="13" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.2105263157895"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="14" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -1980,88 +1852,48 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="51" t="n">
-        <v>8901083012114</v>
-      </c>
-      <c r="D3" s="52" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" s="54" t="n">
+      <c r="B3" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="49" t="n">
+        <v>8901083000838</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="51" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="51" t="n">
-        <v>8901083012121</v>
-      </c>
-      <c r="D4" s="52" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="54" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="56" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="51" t="n">
-        <v>8901083000838</v>
-      </c>
-      <c r="D5" s="56" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="54" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="56" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="51" t="n">
+      <c r="B4" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="49" t="n">
         <v>8901083000845</v>
       </c>
-      <c r="D6" s="56" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" s="54" t="n">
+      <c r="D4" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="51" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A3:A6" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A3:A4" type="list">
       <formula1>"Product Minimum Facings Primary,Product Minimum Facing Secondary "</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>